<commit_message>
Add auto generate xlsx function"
* analyze.py에서 기존의 불러운 값과 새로 만든 dict을 연결하여
  value값들을 연결시켜야 함.
* 그 후 해당 딕셔너리를 dataframe화하여 기존의 misspell_origin.xlsx에
  덤핑해야함
</commit_message>
<xml_diff>
--- a/data/misspell_origin.xlsx
+++ b/data/misspell_origin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijpark\PycharmProjects\mkdg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFB6DFB-841E-470F-9F01-9005525A94EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221BD1DD-1814-40F7-A3CE-737066986989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="2580" windowWidth="13935" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>origin</t>
   </si>
@@ -69,6 +69,22 @@
   </si>
   <si>
     <t>이니라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안녕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헬로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>봉쥬르</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -394,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -448,6 +464,22 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>